<commit_message>
remove unknown services from file
</commit_message>
<xml_diff>
--- a/aspire_upload_example.xlsx
+++ b/aspire_upload_example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Group Name</t>
   </si>
@@ -50,15 +50,6 @@
   </si>
   <si>
     <t>Leaf Removal</t>
-  </si>
-  <si>
-    <t>Seasonal Color</t>
-  </si>
-  <si>
-    <t>Summer Annuals Installation</t>
-  </si>
-  <si>
-    <t>Flowers - Summer Bed Installation</t>
   </si>
 </sst>
 </file>
@@ -389,23 +380,6 @@
         <v>100.0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>